<commit_message>
New Updates to the python script
</commit_message>
<xml_diff>
--- a/Data/Curso1.xlsx
+++ b/Data/Curso1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmalvaez/Library/CloudStorage/GoogleDrive-malvaez.axel@aries.iimas.unam.mx/My Drive/MacBook/Documentos/School/SocialService/AESCULAP/Sentiment-Analysis-Comments-Courses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmalvaez/Library/CloudStorage/GoogleDrive-malvaez.axel@aries.iimas.unam.mx/My Drive/MacBook/Documentos/School/SocialService/AESCULAP/Sentiment-Analysis-Courses/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9A586B-DEAB-3E47-9648-97A9608FE2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CE48E0-5D63-7B47-BDC2-A3C3D449956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{A6AC30B6-096B-6C4A-8497-030C0164802A}"/>
   </bookViews>
@@ -16341,7 +16341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F27391-EE23-2F4A-AEA1-E8A797B1DD84}">
   <dimension ref="A1:A2365"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="113" workbookViewId="0">
       <selection activeCell="A233" sqref="A233"/>
     </sheetView>
   </sheetViews>

</xml_diff>